<commit_message>
MMAUSIHK-12 und MMAUSIHK-6 Erstellung der Zeitbuchung mit Merlin functional
</commit_message>
<xml_diff>
--- a/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
+++ b/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/merlin-testproject/src/main/resources/officeTemplates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/projectforge/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEE2F09-1EC0-B340-BB32-8920D86CB55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF8174-7726-FF43-9393-B9EC956040C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
   </bookViews>
@@ -57,6 +57,13 @@
     <t>#idAllHour</t>
   </si>
   <si>
+    <t>Name und Vorname des Auszubildenen #idName
+#idYear. Ausbildungsjahr
+Ausbildungsnachweis Nr.#idNr
+Für die Woche vom #idFirstDate bis #idLastDate.
+Betrieblicher Funktionsberreich: #idDepartment</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -66,7 +73,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Auszubildene Person</t>
+      <t>Auszubildender</t>
     </r>
     <r>
       <rPr>
@@ -99,7 +106,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Ausbildene Person</t>
+      <t>Ausbildender bzw. Ausbilder</t>
     </r>
     <r>
       <rPr>
@@ -122,19 +129,12 @@
       <t>Datum                                                                 Unterschrift</t>
     </r>
   </si>
-  <si>
-    <t>Name und Vorname des Auszubildenen #idName
-#idYear. Ausbildungsjahr
-Ausbildungsnachweis Nr.#idNr
-Für die Woche vom #idFirstDate bis #idLastDate.
-Betrieblicher Funktionsberreich: #idDepartment</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +183,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -378,7 +385,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -398,6 +404,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -432,10 +441,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,7 +763,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="242" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -767,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="104" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -776,7 +785,7 @@
       <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="30">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -789,37 +798,37 @@
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="13" customFormat="1" ht="14">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:6" s="12" customFormat="1" ht="14">
+      <c r="A3" s="9"/>
       <c r="B3" s="25"/>
       <c r="C3" s="26"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" ht="11">
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="15">
       <c r="A4" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="76" customHeight="1" thickBot="1">
       <c r="A5" s="21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>

</xml_diff>

<commit_message>
Final IHK Export Math
</commit_message>
<xml_diff>
--- a/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
+++ b/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/projectforge/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF8174-7726-FF43-9393-B9EC956040C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C78E5-0875-2745-BDB1-50AFD7E65684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
   </bookViews>
@@ -57,13 +57,6 @@
     <t>#idAllHour</t>
   </si>
   <si>
-    <t>Name und Vorname des Auszubildenen #idName
-#idYear. Ausbildungsjahr
-Ausbildungsnachweis Nr.#idNr
-Für die Woche vom #idFirstDate bis #idLastDate.
-Betrieblicher Funktionsberreich: #idDepartment</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -128,6 +121,13 @@
       </rPr>
       <t>Datum                                                                 Unterschrift</t>
     </r>
+  </si>
+  <si>
+    <t>Name und Vorname des Auszubildenen #idName
+#idYear. Ausbildungsjahr
+Ausbildungsnachweis Nr. #idNr
+Für die Woche vom #idFirstDate bis #idLastDate.
+Betrieblicher Funktionsberreich: #idDepartment</t>
   </si>
 </sst>
 </file>
@@ -763,7 +763,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="242" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -776,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="104" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -824,11 +824,11 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="76" customHeight="1" thickBot="1">
       <c r="A5" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>

</xml_diff>

<commit_message>
Ihk less manuality (#141)
* Added UserComment AusbildungsConfig intake

* Added some Math for DocNr

* Final IHK Export Math

* Fixing UId Bug

* Fixed IHK JSON reading bug

Co-authored-by: jhpeters <jhpeters@micromata.de>
Co-authored-by: Michael Weishaar <m.weishaar@micromata.de>
</commit_message>
<xml_diff>
--- a/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
+++ b/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/projectforge/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF8174-7726-FF43-9393-B9EC956040C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C78E5-0875-2745-BDB1-50AFD7E65684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
   </bookViews>
@@ -57,13 +57,6 @@
     <t>#idAllHour</t>
   </si>
   <si>
-    <t>Name und Vorname des Auszubildenen #idName
-#idYear. Ausbildungsjahr
-Ausbildungsnachweis Nr.#idNr
-Für die Woche vom #idFirstDate bis #idLastDate.
-Betrieblicher Funktionsberreich: #idDepartment</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -128,6 +121,13 @@
       </rPr>
       <t>Datum                                                                 Unterschrift</t>
     </r>
+  </si>
+  <si>
+    <t>Name und Vorname des Auszubildenen #idName
+#idYear. Ausbildungsjahr
+Ausbildungsnachweis Nr. #idNr
+Für die Woche vom #idFirstDate bis #idLastDate.
+Betrieblicher Funktionsberreich: #idDepartment</t>
   </si>
 </sst>
 </file>
@@ -763,7 +763,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="242" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -776,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="104" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -824,11 +824,11 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="76" customHeight="1" thickBot="1">
       <c r="A5" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>

</xml_diff>

<commit_message>
ihk plugin added new template
</commit_message>
<xml_diff>
--- a/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
+++ b/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/projectforge/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mirconuhn/Repositories/projectforge-parent/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C78E5-0875-2745-BDB1-50AFD7E65684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D38938-4583-7445-883E-35422C4EF83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
   </bookViews>
@@ -123,7 +123,7 @@
     </r>
   </si>
   <si>
-    <t>Name und Vorname des Auszubildenen #idName
+    <t>Name und Vorname des Auszubildenden #idName
 #idYear. Ausbildungsjahr
 Ausbildungsnachweis Nr. #idNr
 Für die Woche vom #idFirstDate bis #idLastDate.
@@ -134,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,13 +183,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -360,6 +353,30 @@
       <right style="thin">
         <color theme="1"/>
       </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="1"/>
       </top>
@@ -391,7 +408,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -404,9 +420,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -422,12 +435,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -445,6 +452,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,7 +782,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="242" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -775,23 +794,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="104" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="30">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
@@ -802,37 +821,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" ht="14">
-      <c r="A3" s="9"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
+    <row r="3" spans="1:6" s="11" customFormat="1" ht="14">
+      <c r="A3" s="8"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" ht="15">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="13" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="76" customHeight="1" thickBot="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="24"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="14"/>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="14"/>
@@ -857,10 +876,10 @@
   <mergeCells count="6">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A4:E4"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed name of variables and added error messages in case of (user not found, json not found, wrong json)
</commit_message>
<xml_diff>
--- a/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
+++ b/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mirconuhn/Repositories/projectforge-parent/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/projectforge/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D38938-4583-7445-883E-35422C4EF83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59544B55-1427-BA4A-AC52-F601632D1BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
   </bookViews>
@@ -134,6 +134,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy;@"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -408,18 +411,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -448,13 +454,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -782,7 +785,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="242" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -794,23 +797,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="104" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="30">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
@@ -821,13 +824,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" ht="14">
-      <c r="A3" s="8"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="14">
+      <c r="A3" s="9"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="24" t="s">
@@ -837,21 +840,21 @@
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="26"/>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="76" customHeight="1" thickBot="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="20"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="14"/>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="14"/>

</xml_diff>

<commit_message>
changing calculation of docNr and fixing Document (print and int Lernfeldnummer)
</commit_message>
<xml_diff>
--- a/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
+++ b/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/projectforge/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59544B55-1427-BA4A-AC52-F601632D1BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788AD918-08A4-2846-8334-A874428081CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$F$5</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -123,7 +120,7 @@
     </r>
   </si>
   <si>
-    <t>Name und Vorname des Auszubildenden #idName
+    <t>Name und Vorname des Auszubildenden: #idName
 #idYear. Ausbildungsjahr
 Ausbildungsnachweis Nr. #idNr
 Für die Woche vom #idFirstDate bis #idLastDate.
@@ -392,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -467,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,10 +782,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F2F446-8889-D342-80D4-82351A16B1E6}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="242" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -828,7 +831,7 @@
       <c r="A3" s="9"/>
       <c r="B3" s="22"/>
       <c r="C3" s="23"/>
-      <c r="D3" s="10"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
     </row>
@@ -886,6 +889,6 @@
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="95" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IHK-Plugin added comments and error outputs, fixed mistake in writing of xlsx file
</commit_message>
<xml_diff>
--- a/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
+++ b/plugins/org.projectforge.plugins.ihk/src/main/resources/VorlageWochenbericht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mweishaar/projects/projectforge/plugins/org.projectforge.plugins.ihk/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788AD918-08A4-2846-8334-A874428081CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC909300-54F0-A249-BCCE-CEDD6422B770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
+    <workbookView xWindow="1380" yWindow="500" windowWidth="27560" windowHeight="17540" xr2:uid="{B91F582A-78C6-7145-8887-A5E5397F3E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 #idYear. Ausbildungsjahr
 Ausbildungsnachweis Nr. #idNr
 Für die Woche vom #idFirstDate bis #idLastDate.
-Betrieblicher Funktionsberreich: #idDepartment</t>
+Betrieblicher Funktionsbereich: #idDepartment</t>
   </si>
 </sst>
 </file>
@@ -134,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,6 +423,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -464,9 +467,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,10 +788,10 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="242" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" customWidth="1"/>
@@ -799,24 +799,24 @@
     <col min="4" max="6" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="104" customHeight="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="30">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
@@ -827,57 +827,57 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="14">
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="27"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="76" customHeight="1" thickBot="1">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="21"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="14"/>
-    <row r="17" s="2" customFormat="1" ht="14"/>
-    <row r="18" s="2" customFormat="1" ht="14"/>
-    <row r="19" s="2" customFormat="1" ht="14"/>
-    <row r="20" s="2" customFormat="1" ht="14"/>
-    <row r="21" s="2" customFormat="1" ht="14"/>
-    <row r="22" s="2" customFormat="1" ht="14"/>
-    <row r="23" s="2" customFormat="1" ht="14"/>
-    <row r="24" s="2" customFormat="1" ht="14"/>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="17" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="21" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="23" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="24" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:F1"/>

</xml_diff>